<commit_message>
Adding components for EPV builds in Erythyro- ; Proto- ; Amdo;
</commit_message>
<xml_diff>
--- a/tabular/genus/erythyro-refseqs-side-data.xlsx
+++ b/tabular/genus/erythyro-refseqs-side-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4042EC-B3A1-2149-B2DE-D9F15C9ECC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A843E1B2-6460-AB45-87DA-D431A021A385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>accession-ID</t>
   </si>
@@ -126,10 +126,19 @@
     <t>BPV3</t>
   </si>
   <si>
-    <t>Erythroparvovirus</t>
-  </si>
-  <si>
     <t>NK</t>
+  </si>
+  <si>
+    <t>Ungulate erythroparvovirus 2</t>
+  </si>
+  <si>
+    <t>GiEPV</t>
+  </si>
+  <si>
+    <t>Erythyroparvovirus</t>
+  </si>
+  <si>
+    <t>ErthryoPV-Giraffe-1</t>
   </si>
 </sst>
 </file>
@@ -2376,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A2:B8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2444,28 +2453,28 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L2" t="b">
         <v>0</v>
@@ -2482,28 +2491,28 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>
@@ -2520,28 +2529,28 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L4" t="b">
         <v>0</v>
@@ -2558,28 +2567,28 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
@@ -2596,28 +2605,28 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6" t="b">
         <v>0</v>
@@ -2634,28 +2643,28 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -2672,30 +2681,68 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" t="b">
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Incorporated novel erythyroparvoviruses (hyaena & giraffe) from WGS mining
</commit_message>
<xml_diff>
--- a/tabular/genus/erythyro-refseqs-side-data.xlsx
+++ b/tabular/genus/erythyro-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A843E1B2-6460-AB45-87DA-D431A021A385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F680267-603B-974A-ACE2-A5F54B61B688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18380" yWindow="2760" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REFSET" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>accession-ID</t>
   </si>
@@ -138,7 +138,22 @@
     <t>Erythyroparvovirus</t>
   </si>
   <si>
-    <t>ErthryoPV-Giraffe-1</t>
+    <t>ErythyroPV-Giraffe-1</t>
+  </si>
+  <si>
+    <t>ErythyroPV-Hyaena-1</t>
+  </si>
+  <si>
+    <t>Giraffa camelopardalis</t>
+  </si>
+  <si>
+    <t>Hyaena hyaena</t>
+  </si>
+  <si>
+    <t>Homo sapiens</t>
+  </si>
+  <si>
+    <t>HhEPV</t>
   </si>
 </sst>
 </file>
@@ -2385,15 +2400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C7" sqref="A1:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="7" width="18.6640625" customWidth="1"/>
@@ -2491,7 +2506,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>33</v>
@@ -2719,7 +2734,7 @@
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -2743,6 +2758,44 @@
         <v>33</v>
       </c>
       <c r="L9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>